<commit_message>
1. Fix the column visible model incorrect share bug
This bug is caused by child controller incorrectly share data model.

2. When add, make necessary columns visible.
</commit_message>
<xml_diff>
--- a/management/src/main/resources/Bids_template.xlsx
+++ b/management/src/main/resources/Bids_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="3660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="4740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,13 +108,13 @@
     <t>${record.description}</t>
   </si>
   <si>
-    <t>${record.price}</t>
-  </si>
-  <si>
     <t>${record.salesPersonFullName}</t>
   </si>
   <si>
     <t>${record.productNamesString}</t>
+  </si>
+  <si>
+    <t>${record.biddingPrice}</t>
   </si>
 </sst>
 </file>
@@ -535,16 +535,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>